<commit_message>
added content to results section.
</commit_message>
<xml_diff>
--- a/model_results.xlsx
+++ b/model_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\Uni\2023\DATA3888\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian D02\Desktop\projects\image6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D144451-DA22-4EBD-AA31-DC075F576C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360779AA-F9E8-442F-A383-713C62CF37DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="4" xr2:uid="{ECB30751-74C6-456D-A9C8-72B309C480EE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{ECB30751-74C6-456D-A9C8-72B309C480EE}"/>
   </bookViews>
   <sheets>
     <sheet name="All results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Combined" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="48">
   <si>
     <t>2000 w/class weights</t>
   </si>
@@ -183,14 +182,18 @@
   <si>
     <t>Combined Model</t>
   </si>
+  <si>
+    <t>Table Summary of Validation Loss for Every CNN Model</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -209,12 +212,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -258,16 +267,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -286,9 +292,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -297,15 +305,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -320,6 +319,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,8 +447,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="343648" y="2103296"/>
-          <a:ext cx="10863412" cy="6648661"/>
+          <a:off x="343648" y="2172318"/>
+          <a:ext cx="10449281" cy="6955117"/>
           <a:chOff x="14238869" y="1132249"/>
           <a:chExt cx="13113143" cy="11019062"/>
         </a:xfrm>
@@ -632,8 +714,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11464997" y="2224390"/>
-          <a:ext cx="11548231" cy="6709784"/>
+          <a:off x="11009454" y="2301695"/>
+          <a:ext cx="11597926" cy="7016240"/>
           <a:chOff x="12346512" y="1664727"/>
           <a:chExt cx="12225988" cy="10986909"/>
         </a:xfrm>
@@ -877,8 +959,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="23922245" y="2271505"/>
-          <a:ext cx="10708116" cy="6554053"/>
+          <a:off x="23521918" y="2348810"/>
+          <a:ext cx="10807508" cy="6852226"/>
           <a:chOff x="24076941" y="2401455"/>
           <a:chExt cx="11962404" cy="11233727"/>
         </a:xfrm>
@@ -1127,8 +1209,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="36779916" y="3238408"/>
-          <a:ext cx="12202866" cy="10748241"/>
+          <a:off x="36090709" y="3238408"/>
+          <a:ext cx="12047988" cy="10748241"/>
           <a:chOff x="36380331" y="3126896"/>
           <a:chExt cx="12032500" cy="11017729"/>
         </a:xfrm>
@@ -1372,8 +1454,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="783628" y="2099607"/>
-          <a:ext cx="11904551" cy="10538442"/>
+          <a:off x="775884" y="2099607"/>
+          <a:ext cx="11532843" cy="10538442"/>
           <a:chOff x="775110" y="2150717"/>
           <a:chExt cx="11854215" cy="10803283"/>
         </a:xfrm>
@@ -1617,8 +1699,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="18640288" y="2601951"/>
-          <a:ext cx="12095743" cy="10578805"/>
+          <a:off x="18183397" y="2601951"/>
+          <a:ext cx="11940866" cy="10578805"/>
           <a:chOff x="18496251" y="2667000"/>
           <a:chExt cx="11925378" cy="10839000"/>
         </a:xfrm>
@@ -1867,8 +1949,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="17732523" y="2207664"/>
-          <a:ext cx="12135971" cy="10486401"/>
+          <a:off x="17296332" y="2243271"/>
+          <a:ext cx="12023214" cy="10655537"/>
           <a:chOff x="17573625" y="2286000"/>
           <a:chExt cx="11983749" cy="10858500"/>
         </a:xfrm>
@@ -2112,8 +2194,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="30615636" y="2207664"/>
-          <a:ext cx="12009008" cy="10486401"/>
+          <a:off x="30054818" y="2243271"/>
+          <a:ext cx="11896251" cy="10655537"/>
           <a:chOff x="30288492" y="2286000"/>
           <a:chExt cx="11856786" cy="10858500"/>
         </a:xfrm>
@@ -2357,8 +2439,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="611262" y="1888083"/>
-          <a:ext cx="12785351" cy="11036136"/>
+          <a:off x="605327" y="1917756"/>
+          <a:ext cx="12402571" cy="11214174"/>
           <a:chOff x="611909" y="1895636"/>
           <a:chExt cx="12780819" cy="11081455"/>
         </a:xfrm>
@@ -2670,22 +2752,6 @@
     <tableColumn id="5" xr3:uid="{60FDF158-5E34-4F3F-91A1-19F6DEAC9460}" name="2000 w/categorical crossentropy &amp; class weights"/>
     <tableColumn id="6" xr3:uid="{C373AAB4-0947-42E8-9057-A11B854587CD}" name="2000 w/RMSprop"/>
     <tableColumn id="7" xr3:uid="{5F75518B-E1D6-4E66-AA67-BB230347B20E}" name="2000 w/RMSprop &amp; class weights"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{9D580DEC-9162-4292-A78C-5436DC733F20}" name="Table2456789111424" displayName="Table2456789111424" ref="C33:I35" totalsRowShown="0">
-  <autoFilter ref="C33:I35" xr:uid="{9D580DEC-9162-4292-A78C-5436DC733F20}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9F31703B-E34C-4923-94B1-BBCAC68600F4}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{A4805BE2-97AB-4F91-8545-1738A907B522}" name="2000"/>
-    <tableColumn id="3" xr3:uid="{72410AE9-5723-4F19-86E0-DEDDABF54551}" name="2000 w/class weights"/>
-    <tableColumn id="4" xr3:uid="{695AB1B4-0E0C-475B-A240-3EEC3360D490}" name="2000 w/categorical crossentropy"/>
-    <tableColumn id="5" xr3:uid="{241B96A6-C423-4FB6-BE0B-C2CEC15EB154}" name="2000 w/categorical crossentropy &amp; class weights"/>
-    <tableColumn id="6" xr3:uid="{EE9221D9-929F-469E-AFB8-B54039854247}" name="2000 w/RMSprop"/>
-    <tableColumn id="7" xr3:uid="{78C8A3B8-E114-4266-8368-3F87836B7CC4}" name="2000 w/RMSprop &amp; class weights"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3122,17 +3188,17 @@
       <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" customWidth="1"/>
-    <col min="3" max="3" width="20.36328125" customWidth="1"/>
-    <col min="4" max="4" width="29.90625" customWidth="1"/>
-    <col min="5" max="5" width="43.08984375" customWidth="1"/>
-    <col min="6" max="6" width="41.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.08984375" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="5" max="5" width="43.140625" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3155,7 +3221,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3178,7 +3244,7 @@
         <v>0.15989999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3201,15 +3267,15 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3232,7 +3298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3255,7 +3321,7 @@
         <v>0.19009999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -3278,12 +3344,12 @@
         <v>9.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -3306,7 +3372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -3329,7 +3395,7 @@
         <v>0.1842</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -3352,12 +3418,12 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -3380,7 +3446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -3403,7 +3469,7 @@
         <v>0.17699999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -3426,12 +3492,12 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -3454,7 +3520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -3477,7 +3543,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -3500,12 +3566,12 @@
         <v>8.7499999999999994E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -3528,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -3551,7 +3617,7 @@
         <v>0.1585</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -3574,12 +3640,12 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -3602,7 +3668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -3625,7 +3691,7 @@
         <v>0.1721</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -3648,15 +3714,15 @@
         <v>8.2500000000000004E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -3679,7 +3745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -3702,7 +3768,7 @@
         <v>0.15909999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -3725,12 +3791,12 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -3753,7 +3819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -3776,7 +3842,7 @@
         <v>0.1608</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -3799,18 +3865,18 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -3833,7 +3899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -3856,7 +3922,7 @@
         <v>0.16239999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -3879,12 +3945,12 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -3907,7 +3973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -3930,7 +3996,7 @@
         <v>0.1646</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -3953,12 +4019,12 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -3981,7 +4047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -4004,7 +4070,7 @@
         <v>0.16020000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -4027,12 +4093,12 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -4055,23 +4121,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>3</v>
       </c>
       <c r="B75" s="3"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>4</v>
       </c>
@@ -4094,7 +4160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -4117,7 +4183,7 @@
         <v>0.15579999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -4170,266 +4236,266 @@
       <selection activeCell="B3" sqref="B3:N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" customWidth="1"/>
-    <col min="9" max="9" width="17.1796875" customWidth="1"/>
-    <col min="10" max="10" width="18.81640625" customWidth="1"/>
-    <col min="11" max="11" width="11.26953125" customWidth="1"/>
-    <col min="12" max="12" width="13.90625" customWidth="1"/>
-    <col min="13" max="13" width="11.6328125" customWidth="1"/>
-    <col min="14" max="14" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B3" s="15" t="s">
+    <row r="1" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18" t="s">
+      <c r="J3" s="13"/>
+      <c r="K3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18" t="s">
+      <c r="L3" s="13"/>
+      <c r="M3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="18"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="16"/>
-      <c r="C4" s="8" t="s">
+      <c r="N3" s="13"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>0.2298</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>0.185</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>0.11</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>6.1524000000000001</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>5.5162000000000004</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="7">
         <v>9.69E-2</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="7">
         <v>0.17180000000000001</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="7">
         <v>0.1</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="7">
         <v>0.15989999999999999</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <v>0.09</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="9">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
         <v>0.2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>0.2238</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>0.21879999999999999</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>0.08</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <v>6.7022000000000004</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>0.09</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>6.1444999999999999</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>0.08</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>0.23730000000000001</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
         <v>0.10249999999999999</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <v>0.19009999999999999</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="6">
         <v>9.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>0.8</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>0.26069999999999999</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>0.2094</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>0.08</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>6.6276000000000002</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>6.25E-2</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>6.3433999999999999</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <v>0.20419999999999999</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <v>0.09</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="7">
         <v>0.17699999999999999</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>0.30780000000000002</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>0.20860000000000001</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>6.8411999999999997</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>0.10249999999999999</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>6.1580000000000004</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="7">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="7">
         <v>0.21490000000000001</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="7">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="7">
         <v>0.18</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="7">
         <v>8.7499999999999994E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
   </sheetData>
@@ -4456,255 +4522,255 @@
       <selection activeCell="AV35" sqref="AV35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.1796875" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" customWidth="1"/>
-    <col min="10" max="10" width="25.1796875" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" customWidth="1"/>
-    <col min="14" max="14" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18" t="s">
+      <c r="L4" s="13"/>
+      <c r="M4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="18"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="16"/>
-      <c r="C5" s="8" t="s">
+      <c r="N4" s="13"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
+      <c r="C5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>0.2298</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>0.185</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>0.11</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>6.1524000000000001</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>5.5162000000000004</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <v>9.69E-2</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="7">
         <v>0.17180000000000001</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="7">
         <v>0.1</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="7">
         <v>0.15989999999999999</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <v>0.09</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="9">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
         <v>90</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.2334</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>9.7500000000000003E-2</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>0.19439999999999999</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>5.5658000000000003</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>4.8395000000000001</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>0.09</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>0.1842</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <v>0.09</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <v>0.16239999999999999</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="6">
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="10">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
         <v>180</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>0.1807</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>0.1</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>0.1794</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>5.5938999999999997</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <v>0.10249999999999999</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="7">
         <v>4.9142000000000001</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="7">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="7">
         <v>0.17710000000000001</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="7">
         <v>0.105</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="7">
         <v>0.1646</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="7">
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>0.26069999999999999</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>7.7499999999999999E-2</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>0.184</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>5.9652000000000003</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>0.115</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>5.1211000000000002</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="7">
         <v>7.7499999999999999E-2</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="7">
         <v>0.18129999999999999</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="7">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="7">
         <v>0.16020000000000001</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
     </row>
   </sheetData>
@@ -4730,259 +4796,259 @@
       <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" customWidth="1"/>
-    <col min="7" max="7" width="15.08984375" customWidth="1"/>
-    <col min="10" max="10" width="20.7265625" customWidth="1"/>
-    <col min="11" max="11" width="20.90625" customWidth="1"/>
-    <col min="14" max="14" width="13.54296875" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C5" s="15" t="s">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18" t="s">
+      <c r="I5" s="13"/>
+      <c r="J5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18" t="s">
+      <c r="K5" s="13"/>
+      <c r="L5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18" t="s">
+      <c r="M5" s="13"/>
+      <c r="N5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="18"/>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C6" s="16"/>
-      <c r="D6" s="8" t="s">
+      <c r="O5" s="13"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" s="15"/>
+      <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C7" s="8" t="s">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>0.2298</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>0.185</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>0.11</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>6.1524000000000001</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <v>5.5162000000000004</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <v>9.69E-2</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <v>0.17180000000000001</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="7">
         <v>0.1</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <v>0.15989999999999999</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="7">
         <v>0.09</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C8" s="9" t="s">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>0.21840000000000001</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>0.1739</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>5.8</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>0.11749999999999999</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <v>5.2885999999999997</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>0.09</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="6">
         <v>0.16830000000000001</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <v>0.105</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="6">
         <v>0.1585</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="6">
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C9" s="12" t="s">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>0.22040000000000001</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>0.1075</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>0.17730000000000001</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>5.0793999999999997</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="7">
         <v>4.6886999999999999</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="7">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="7">
         <v>0.17319999999999999</v>
       </c>
-      <c r="M9" s="8">
+      <c r="M9" s="7">
         <v>0.11</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <v>0.1721</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="7">
         <v>8.2500000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C10" s="11" t="s">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>0.21759999999999999</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>0.16719999999999999</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <v>4.9836</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <v>8.2500000000000004E-2</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="7">
         <v>4.3703000000000003</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="7">
         <v>0.105</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="7">
         <v>0.16980000000000001</v>
       </c>
-      <c r="M10" s="8">
+      <c r="M10" s="7">
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="7">
         <v>0.15909999999999999</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10" s="7">
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="3"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="3"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
     </row>
   </sheetData>
@@ -5002,980 +5068,1047 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BB7E86-6324-49FA-994D-1032292C2DAC}">
-  <dimension ref="B4:O35"/>
+  <dimension ref="B2:X35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13:O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.6328125" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" customWidth="1"/>
-    <col min="11" max="11" width="11.81640625" customWidth="1"/>
-    <col min="14" max="14" width="13.81640625" customWidth="1"/>
-    <col min="15" max="15" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="D4" s="17" t="s">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="G2" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17" t="s">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17" t="s">
+      <c r="G4" s="16"/>
+      <c r="H4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17" t="s">
+      <c r="K4" s="16"/>
+      <c r="L4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17" t="s">
+      <c r="M4" s="16"/>
+      <c r="N4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="17"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="D5" t="s">
+      <c r="O4" s="16"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="D5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="25"/>
+      <c r="F5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="G5" s="25"/>
+      <c r="H5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="I5" s="25"/>
+      <c r="J5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="K5" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="K5" s="25"/>
+      <c r="L5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="M5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="M5" s="25"/>
+      <c r="N5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="O5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B6" s="19" t="s">
+      <c r="O5" s="25"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="8">
+      <c r="C6" s="21"/>
+      <c r="D6" s="21">
         <v>0.2298</v>
       </c>
-      <c r="E6" s="8">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="E6" s="21"/>
+      <c r="F6" s="21">
         <v>0.185</v>
       </c>
-      <c r="G6" s="8">
-        <v>0.11</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="G6" s="21"/>
+      <c r="H6" s="21">
         <v>6.1524000000000001</v>
       </c>
-      <c r="I6" s="8">
-        <v>7.8100000000000003E-2</v>
-      </c>
-      <c r="J6" s="8">
+      <c r="I6" s="21"/>
+      <c r="J6" s="21">
         <v>5.5162000000000004</v>
       </c>
-      <c r="K6" s="8">
-        <v>9.69E-2</v>
-      </c>
-      <c r="L6" s="8">
+      <c r="K6" s="21"/>
+      <c r="L6" s="21">
         <v>0.17180000000000001</v>
       </c>
-      <c r="M6" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="N6" s="8">
+      <c r="M6" s="21"/>
+      <c r="N6" s="21">
         <v>0.15989999999999999</v>
       </c>
-      <c r="O6" s="8">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B7" s="21" t="s">
+      <c r="O6" s="21"/>
+      <c r="Q6">
+        <f>D6-F6</f>
+        <v>4.4800000000000006E-2</v>
+      </c>
+      <c r="R6">
+        <f>Q6/D6</f>
+        <v>0.19495213228894692</v>
+      </c>
+      <c r="T6">
+        <f>D6-L6</f>
+        <v>5.7999999999999996E-2</v>
+      </c>
+      <c r="U6">
+        <f>T6/D6</f>
+        <v>0.25239338555265445</v>
+      </c>
+      <c r="W6">
+        <f>F6-N6</f>
+        <v>2.5100000000000011E-2</v>
+      </c>
+      <c r="X6">
+        <f>W6/F6</f>
+        <v>0.13567567567567573</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="26">
         <v>0.2</v>
       </c>
-      <c r="D7" s="13">
-        <v>0.2238</v>
-      </c>
-      <c r="E7" s="13">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="F7" s="13">
-        <v>0.21879999999999999</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0.08</v>
-      </c>
-      <c r="H7" s="13">
-        <v>6.7022000000000004</v>
-      </c>
-      <c r="I7" s="13">
-        <v>0.09</v>
-      </c>
-      <c r="J7" s="13">
-        <v>6.1444999999999999</v>
-      </c>
-      <c r="K7" s="13">
-        <v>0.08</v>
-      </c>
-      <c r="L7" s="13">
-        <v>0.23730000000000001</v>
-      </c>
-      <c r="M7" s="13">
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="N7" s="13">
-        <v>0.19009999999999999</v>
-      </c>
-      <c r="O7" s="13">
-        <v>9.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B8" s="15"/>
+      <c r="D7" s="35">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="E7" s="35"/>
+      <c r="F7" s="27">
+        <v>0.2029</v>
+      </c>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27">
+        <v>6.2573999999999996</v>
+      </c>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27">
+        <v>5.8756000000000004</v>
+      </c>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27">
+        <v>0.22020000000000001</v>
+      </c>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27">
+        <v>0.18210000000000001</v>
+      </c>
+      <c r="O7" s="27"/>
+      <c r="Q7">
+        <f t="shared" ref="Q7:Q16" si="0">D7-F7</f>
+        <v>9.0099999999999986E-2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7:R16" si="1">Q7/D7</f>
+        <v>0.30750853242320814</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ref="T7:T16" si="2">D7-L7</f>
+        <v>7.2799999999999976E-2</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7:U16" si="3">T7/D7</f>
+        <v>0.24846416382252554</v>
+      </c>
+      <c r="W7">
+        <f t="shared" ref="W7:W16" si="4">F7-N7</f>
+        <v>2.0799999999999985E-2</v>
+      </c>
+      <c r="X7">
+        <f t="shared" ref="X7:X16" si="5">W7/F7</f>
+        <v>0.10251355347461796</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
       <c r="C8">
         <v>0.8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="42">
         <v>0.26069999999999999</v>
       </c>
-      <c r="E8">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="F8">
-        <v>0.2094</v>
-      </c>
-      <c r="G8">
-        <v>0.08</v>
-      </c>
-      <c r="H8">
+      <c r="E8" s="42"/>
+      <c r="F8" s="36">
+        <v>0.221</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="23">
         <v>6.6276000000000002</v>
       </c>
-      <c r="I8">
-        <v>6.25E-2</v>
-      </c>
-      <c r="J8">
+      <c r="I8" s="23"/>
+      <c r="J8" s="23">
         <v>6.3433999999999999</v>
       </c>
-      <c r="K8">
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="L8">
-        <v>0.20419999999999999</v>
-      </c>
-      <c r="M8">
-        <v>0.09</v>
-      </c>
-      <c r="N8">
+      <c r="K8" s="23"/>
+      <c r="L8" s="23">
+        <v>0.21560000000000001</v>
+      </c>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23">
+        <v>0.17510000000000001</v>
+      </c>
+      <c r="O8" s="23"/>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>3.9699999999999985E-2</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>0.15228231683927881</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="2"/>
+        <v>4.5099999999999973E-2</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="3"/>
+        <v>0.17299578059071721</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="4"/>
+        <v>4.5899999999999996E-2</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="5"/>
+        <v>0.20769230769230768</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="29">
+        <v>0.30780000000000002</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29">
+        <v>0.20860000000000001</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29">
+        <v>6.8411999999999997</v>
+      </c>
+      <c r="I9" s="29"/>
+      <c r="J9" s="37">
+        <v>6.4580000000000002</v>
+      </c>
+      <c r="K9" s="37"/>
+      <c r="L9" s="29">
+        <v>0.21490000000000001</v>
+      </c>
+      <c r="M9" s="29"/>
+      <c r="N9" s="37">
+        <v>0.18</v>
+      </c>
+      <c r="O9" s="37"/>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>9.920000000000001E-2</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>0.32228719948018197</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>9.290000000000001E-2</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="3"/>
+        <v>0.30181936322287201</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="4"/>
+        <v>2.8600000000000014E-2</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="5"/>
+        <v>0.13710450623202308</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="22">
+        <v>0.21010000000000001</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="38">
         <v>0.17699999999999999</v>
       </c>
-      <c r="O8">
-        <v>6.5000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="16"/>
-      <c r="C9" s="6" t="s">
+      <c r="G10" s="38"/>
+      <c r="H10" s="38">
+        <v>5.6170999999999998</v>
+      </c>
+      <c r="I10" s="38"/>
+      <c r="J10" s="22">
+        <v>4.7255000000000003</v>
+      </c>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22">
+        <v>0.1782</v>
+      </c>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22">
+        <v>0.15629999999999999</v>
+      </c>
+      <c r="O10" s="22"/>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>3.3100000000000018E-2</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>0.15754402665397438</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>3.1900000000000012E-2</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="3"/>
+        <v>0.15183246073298434</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="4"/>
+        <v>2.0699999999999996E-2</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="5"/>
+        <v>0.11694915254237287</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="30">
+        <v>0.2145</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30">
+        <v>0.1714</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="39">
+        <v>5.1790000000000003</v>
+      </c>
+      <c r="I11" s="39"/>
+      <c r="J11" s="30">
+        <v>4.4703999999999997</v>
+      </c>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30">
+        <v>0.16520000000000001</v>
+      </c>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30">
+        <v>0.15920000000000001</v>
+      </c>
+      <c r="O11" s="30"/>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>0.20093240093240095</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="2"/>
+        <v>4.9299999999999983E-2</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="3"/>
+        <v>0.22983682983682976</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="4"/>
+        <v>1.2199999999999989E-2</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="5"/>
+        <v>7.11785297549591E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="7">
-        <v>0.30780000000000002</v>
-      </c>
-      <c r="E9" s="7">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0.20860000000000001</v>
-      </c>
-      <c r="G9" s="7">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H9" s="7">
-        <v>6.8411999999999997</v>
-      </c>
-      <c r="I9" s="7">
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="J9" s="7">
-        <v>6.1580000000000004</v>
-      </c>
-      <c r="K9" s="7">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="L9" s="7">
-        <v>0.21490000000000001</v>
-      </c>
-      <c r="M9" s="7">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="N9" s="7">
-        <v>0.18</v>
-      </c>
-      <c r="O9" s="7">
-        <v>8.7499999999999994E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B10" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10">
-        <v>0.21840000000000001</v>
-      </c>
-      <c r="E10">
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="F10">
-        <v>0.1739</v>
-      </c>
-      <c r="G10">
-        <v>7.2499999999999995E-2</v>
-      </c>
-      <c r="H10">
+      <c r="D12" s="24">
+        <v>0.26069999999999999</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="40">
+        <v>0.184</v>
+      </c>
+      <c r="G12" s="40"/>
+      <c r="H12" s="24">
+        <v>5.9652000000000003</v>
+      </c>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24">
+        <v>5.1211000000000002</v>
+      </c>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24">
+        <v>0.18129999999999999</v>
+      </c>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24">
+        <v>0.16020000000000001</v>
+      </c>
+      <c r="O12" s="24"/>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>7.669999999999999E-2</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>0.29420790180283851</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>7.9399999999999998E-2</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="3"/>
+        <v>0.30456463367855774</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="4"/>
+        <v>2.3799999999999988E-2</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="5"/>
+        <v>0.12934782608695647</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="32">
+        <v>90</v>
+      </c>
+      <c r="D13" s="27">
+        <v>0.23549999999999999</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27">
+        <v>0.18779999999999999</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="34">
         <v>5.8</v>
       </c>
-      <c r="I10">
-        <v>0.11749999999999999</v>
-      </c>
-      <c r="J10">
-        <v>5.2885999999999997</v>
-      </c>
-      <c r="K10">
-        <v>0.09</v>
-      </c>
-      <c r="L10">
-        <v>0.16830000000000001</v>
-      </c>
-      <c r="M10">
-        <v>0.105</v>
-      </c>
-      <c r="N10">
-        <v>0.1585</v>
-      </c>
-      <c r="O10">
-        <v>6.5000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>0.22040000000000001</v>
-      </c>
-      <c r="E11">
-        <v>0.1075</v>
-      </c>
-      <c r="F11">
-        <v>0.17730000000000001</v>
-      </c>
-      <c r="G11">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="H11">
-        <v>5.0793999999999997</v>
-      </c>
-      <c r="I11">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="J11">
-        <v>4.6886999999999999</v>
-      </c>
-      <c r="K11">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="L11">
-        <v>0.17319999999999999</v>
-      </c>
-      <c r="M11">
-        <v>0.11</v>
-      </c>
-      <c r="N11">
-        <v>0.1721</v>
-      </c>
-      <c r="O11">
-        <v>8.2500000000000004E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B12" s="16"/>
-      <c r="C12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0.21759999999999999</v>
-      </c>
-      <c r="E12" s="7">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0.16719999999999999</v>
-      </c>
-      <c r="G12" s="7">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="H12" s="7">
-        <v>4.9836</v>
-      </c>
-      <c r="I12" s="7">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="J12" s="7">
-        <v>4.3703000000000003</v>
-      </c>
-      <c r="K12" s="7">
-        <v>0.105</v>
-      </c>
-      <c r="L12" s="7">
-        <v>0.16980000000000001</v>
-      </c>
-      <c r="M12" s="7">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="N12" s="7">
-        <v>0.15909999999999999</v>
-      </c>
-      <c r="O12" s="7">
-        <v>5.5E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B13" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13">
-        <v>90</v>
-      </c>
-      <c r="D13">
-        <v>0.2334</v>
-      </c>
-      <c r="E13">
-        <v>9.7500000000000003E-2</v>
-      </c>
-      <c r="F13">
-        <v>0.19439999999999999</v>
-      </c>
-      <c r="G13">
-        <v>6.7500000000000004E-2</v>
-      </c>
-      <c r="H13">
-        <v>5.5658000000000003</v>
-      </c>
-      <c r="I13">
-        <v>6.7500000000000004E-2</v>
-      </c>
-      <c r="J13">
-        <v>4.8395000000000001</v>
-      </c>
-      <c r="K13">
-        <v>0.09</v>
-      </c>
-      <c r="L13">
-        <v>0.1842</v>
-      </c>
-      <c r="M13">
-        <v>0.09</v>
-      </c>
-      <c r="N13">
-        <v>0.16239999999999999</v>
-      </c>
-      <c r="O13">
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B14" s="23"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="27">
+        <v>5.2267000000000001</v>
+      </c>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27">
+        <v>0.1628</v>
+      </c>
+      <c r="O13" s="27"/>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>4.7699999999999992E-2</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>0.20254777070063693</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>5.3199999999999997E-2</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="3"/>
+        <v>0.22590233545647559</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="4"/>
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="5"/>
+        <v>0.13312034078807239</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
       <c r="C14">
         <v>180</v>
       </c>
-      <c r="D14">
-        <v>0.1807</v>
-      </c>
-      <c r="E14">
-        <v>0.1</v>
-      </c>
-      <c r="F14">
-        <v>0.1794</v>
-      </c>
-      <c r="G14">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="H14">
-        <v>5.5938999999999997</v>
-      </c>
-      <c r="I14">
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="J14">
-        <v>4.9142000000000001</v>
-      </c>
-      <c r="K14">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="L14">
-        <v>0.17710000000000001</v>
-      </c>
-      <c r="M14">
-        <v>0.105</v>
-      </c>
-      <c r="N14">
-        <v>0.1646</v>
-      </c>
-      <c r="O14">
-        <v>6.7500000000000004E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B15" s="24"/>
-      <c r="C15" s="6" t="s">
+      <c r="D14" s="36">
+        <v>0.246</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="23">
+        <v>0.18360000000000001</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="41">
+        <v>5.6346999999999996</v>
+      </c>
+      <c r="I14" s="41"/>
+      <c r="J14" s="23">
+        <v>4.9477000000000002</v>
+      </c>
+      <c r="K14" s="23"/>
+      <c r="L14" s="36">
+        <v>0.184</v>
+      </c>
+      <c r="M14" s="36"/>
+      <c r="N14" s="23">
+        <v>0.1585</v>
+      </c>
+      <c r="O14" s="23"/>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>6.2399999999999983E-2</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>0.2536585365853658</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="2"/>
+        <v>6.2E-2</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="3"/>
+        <v>0.25203252032520324</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="4"/>
+        <v>2.5100000000000011E-2</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="5"/>
+        <v>0.13671023965141618</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B15" s="20"/>
+      <c r="C15" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="7">
-        <v>0.26069999999999999</v>
-      </c>
-      <c r="E15" s="7">
-        <v>7.7499999999999999E-2</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0.184</v>
-      </c>
-      <c r="G15" s="7">
-        <v>7.2499999999999995E-2</v>
-      </c>
-      <c r="H15" s="7">
-        <v>5.9652000000000003</v>
-      </c>
-      <c r="I15" s="7">
-        <v>0.115</v>
-      </c>
-      <c r="J15" s="7">
-        <v>5.1211000000000002</v>
-      </c>
-      <c r="K15" s="7">
-        <v>7.7499999999999999E-2</v>
-      </c>
-      <c r="L15" s="7">
-        <v>0.18129999999999999</v>
-      </c>
-      <c r="M15" s="7">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="N15" s="7">
-        <v>0.16020000000000001</v>
-      </c>
-      <c r="O15" s="7">
-        <v>6.5000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="N19" s="18"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B20" s="16"/>
-      <c r="C20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="N20" s="8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B21" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="8">
-        <v>0.2298</v>
-      </c>
-      <c r="D21" s="8">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="E21" s="8">
-        <v>0.185</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0.11</v>
-      </c>
-      <c r="G21" s="8">
-        <v>6.1524000000000001</v>
-      </c>
-      <c r="H21" s="8">
-        <v>7.8100000000000003E-2</v>
-      </c>
-      <c r="I21" s="8">
-        <v>5.5162000000000004</v>
-      </c>
-      <c r="J21" s="8">
-        <v>9.69E-2</v>
-      </c>
-      <c r="K21" s="8">
-        <v>0.17180000000000001</v>
-      </c>
-      <c r="L21" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="M21" s="8">
-        <v>0.15989999999999999</v>
-      </c>
-      <c r="N21" s="8">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B22" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="C22" s="7">
-        <v>0.2238</v>
-      </c>
-      <c r="D22" s="7">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="E22" s="7">
-        <v>0.21879999999999999</v>
-      </c>
-      <c r="F22" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="G22" s="7">
-        <v>6.7022000000000004</v>
-      </c>
-      <c r="H22" s="7">
-        <v>0.09</v>
-      </c>
-      <c r="I22" s="7">
-        <v>6.1444999999999999</v>
-      </c>
-      <c r="J22" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="K22" s="7">
-        <v>0.23730000000000001</v>
-      </c>
-      <c r="L22" s="7">
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="M22" s="7">
-        <v>0.19009999999999999</v>
-      </c>
-      <c r="N22" s="7">
-        <v>9.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B23" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="C23" s="8">
-        <v>0.26069999999999999</v>
-      </c>
-      <c r="D23" s="8">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="E23" s="8">
-        <v>0.2094</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0.08</v>
-      </c>
-      <c r="G23" s="8">
-        <v>6.6276000000000002</v>
-      </c>
-      <c r="H23" s="8">
-        <v>6.25E-2</v>
-      </c>
-      <c r="I23" s="8">
-        <v>6.3433999999999999</v>
-      </c>
-      <c r="J23" s="8">
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="K23" s="8">
-        <v>0.20419999999999999</v>
-      </c>
-      <c r="L23" s="8">
-        <v>0.09</v>
-      </c>
-      <c r="M23" s="8">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="N23" s="8">
-        <v>6.5000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="8">
-        <v>0.30780000000000002</v>
-      </c>
-      <c r="D24" s="8">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="E24" s="8">
-        <v>0.20860000000000001</v>
-      </c>
-      <c r="F24" s="8">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G24" s="8">
-        <v>6.8411999999999997</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0.10249999999999999</v>
-      </c>
-      <c r="I24" s="8">
-        <v>6.1580000000000004</v>
-      </c>
-      <c r="J24" s="8">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="K24" s="8">
-        <v>0.21490000000000001</v>
-      </c>
-      <c r="L24" s="8">
-        <v>8.2500000000000004E-2</v>
-      </c>
-      <c r="M24" s="8">
-        <v>0.18</v>
-      </c>
-      <c r="N24" s="8">
-        <v>8.7499999999999994E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="D26" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="O26" s="17"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" t="s">
-        <v>3</v>
-      </c>
-      <c r="H27" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27" t="s">
-        <v>7</v>
-      </c>
-      <c r="K27" t="s">
-        <v>3</v>
-      </c>
-      <c r="L27" t="s">
-        <v>7</v>
-      </c>
-      <c r="M27" t="s">
-        <v>3</v>
-      </c>
-      <c r="N27" t="s">
-        <v>7</v>
-      </c>
-      <c r="O27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B28" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="8">
-        <v>0.2298</v>
-      </c>
-      <c r="E28" s="8">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="F28" s="8">
-        <v>0.185</v>
-      </c>
-      <c r="G28" s="8">
-        <v>0.11</v>
-      </c>
-      <c r="H28" s="8">
-        <v>6.1524000000000001</v>
-      </c>
-      <c r="I28" s="8">
-        <v>7.8100000000000003E-2</v>
-      </c>
-      <c r="J28" s="8">
-        <v>5.5162000000000004</v>
-      </c>
-      <c r="K28" s="8">
-        <v>9.69E-2</v>
-      </c>
-      <c r="L28" s="8">
-        <v>0.17180000000000001</v>
-      </c>
-      <c r="M28" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="N28" s="8">
-        <v>0.15989999999999999</v>
-      </c>
-      <c r="O28" s="8">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B29" s="20" t="s">
+      <c r="D15" s="29">
+        <v>0.2611</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="G15" s="29"/>
+      <c r="H15" s="37">
+        <v>6.11</v>
+      </c>
+      <c r="I15" s="37"/>
+      <c r="J15" s="29">
+        <v>5.4714</v>
+      </c>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29">
+        <v>0.18240000000000001</v>
+      </c>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29">
+        <v>0.16289999999999999</v>
+      </c>
+      <c r="O15" s="29"/>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>7.9300000000000009E-2</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>0.30371505170432789</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>7.8699999999999992E-2</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="3"/>
+        <v>0.30141708157793945</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="4"/>
+        <v>1.89E-2</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="5"/>
+        <v>0.10396039603960397</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B16" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29">
-        <v>0.20039999999999999</v>
-      </c>
-      <c r="E29">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="F29">
-        <v>0.17180000000000001</v>
-      </c>
-      <c r="G29">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="H29">
-        <v>4.9096000000000002</v>
-      </c>
-      <c r="I29">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="J29">
-        <v>4.1261000000000001</v>
-      </c>
-      <c r="K29">
-        <v>6.25E-2</v>
-      </c>
-      <c r="L29">
-        <v>0.17929999999999999</v>
-      </c>
-      <c r="M29">
-        <v>0.08</v>
-      </c>
-      <c r="N29">
-        <v>0.15579999999999999</v>
-      </c>
-      <c r="O29">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
-        <v>1</v>
-      </c>
-      <c r="G33" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" t="s">
-        <v>6</v>
-      </c>
-      <c r="I33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34">
-        <v>0.20039999999999999</v>
-      </c>
-      <c r="E34">
-        <v>0.17180000000000001</v>
-      </c>
-      <c r="F34">
-        <v>4.9096000000000002</v>
-      </c>
-      <c r="G34">
-        <v>4.1261000000000001</v>
-      </c>
-      <c r="H34">
-        <v>0.17929999999999999</v>
-      </c>
-      <c r="I34">
-        <v>0.15579999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C35" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="3">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="E35">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="F35">
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="G35">
-        <v>6.25E-2</v>
-      </c>
-      <c r="H35">
-        <v>0.08</v>
-      </c>
-      <c r="I35">
-        <v>0.06</v>
-      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22">
+        <v>0.2084</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22">
+        <v>0.1769</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22">
+        <v>4.8067000000000002</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22">
+        <v>4.6177000000000001</v>
+      </c>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22">
+        <v>0.18909999999999999</v>
+      </c>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22">
+        <v>0.16009999999999999</v>
+      </c>
+      <c r="O16" s="22"/>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>3.15E-2</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>0.15115163147792707</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="2"/>
+        <v>1.9300000000000012E-2</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="3"/>
+        <v>9.2610364683301402E-2</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="4"/>
+        <v>1.6800000000000009E-2</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="5"/>
+        <v>9.4968908988128944E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <f>AVERAGE(Q6:Q16)</f>
+        <v>5.8872727272727271E-2</v>
+      </c>
+      <c r="R17">
+        <f>AVERAGE(R6:R16)</f>
+        <v>0.23098068189900792</v>
+      </c>
+      <c r="T17">
+        <f>AVERAGE(T6:T16)</f>
+        <v>5.8418181818181814E-2</v>
+      </c>
+      <c r="U17">
+        <f>AVERAGE(U6:U16)</f>
+        <v>0.23035171995273276</v>
+      </c>
+      <c r="W17">
+        <f>AVERAGE(W6:W16)</f>
+        <v>2.3900000000000001E-2</v>
+      </c>
+      <c r="X17">
+        <f>AVERAGE(X6:X16)</f>
+        <v>0.12447467608419403</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="46"/>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B20" s="43"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B22" s="47"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B23" s="48"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B24" s="49"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+    </row>
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+    </row>
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="46"/>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
+      <c r="N32" s="46"/>
+      <c r="O32" s="46"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
+      <c r="N34" s="46"/>
+      <c r="O34" s="46"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:D19"/>
+  <mergeCells count="97">
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="N26:O26"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="I19:J19"/>
@@ -5986,10 +6119,32 @@
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>